<commit_message>
Support phone number in excel sample
</commit_message>
<xml_diff>
--- a/sources/excel-basic/Exempelfil.xlsx
+++ b/sources/excel-basic/Exempelfil.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\go_import\sources\excel_customertemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\move-to-go\sources\excel-basic\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21000" windowHeight="11988"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21000" windowHeight="11985" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Företag" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="93">
   <si>
     <t>Namn</t>
   </si>
@@ -342,6 +342,15 @@
   </si>
   <si>
     <t>Besöksort</t>
+  </si>
+  <si>
+    <t>DirectPhoneNumber</t>
+  </si>
+  <si>
+    <t>MobilePhoneNumber</t>
+  </si>
+  <si>
+    <t>HomePhoneNumber</t>
   </si>
 </sst>
 </file>
@@ -714,26 +723,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.109375" style="4"/>
+    <col min="10" max="10" width="12.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>70</v>
       </c>
@@ -771,7 +780,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -800,7 +809,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -829,7 +838,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -867,7 +876,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>542</v>
       </c>
@@ -896,7 +905,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>987</v>
       </c>
@@ -946,16 +955,16 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="26.33203125" customWidth="1"/>
-    <col min="6" max="6" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="26.28515625" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -975,7 +984,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -992,7 +1001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1012,7 +1021,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1032,7 +1041,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -1049,7 +1058,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1069,289 +1078,289 @@
         <v>987</v>
       </c>
     </row>
-    <row r="77" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
     </row>
-    <row r="95" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
     </row>
-    <row r="97" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
     </row>
-    <row r="102" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
     </row>
-    <row r="104" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
     </row>
-    <row r="123" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
     </row>
-    <row r="161" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="161" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D161" s="2"/>
       <c r="E161" s="2"/>
     </row>
-    <row r="174" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C174" s="2"/>
       <c r="D174" s="2"/>
       <c r="E174" s="2"/>
     </row>
-    <row r="207" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="207" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C207" s="2"/>
       <c r="D207" s="2"/>
       <c r="E207" s="2"/>
     </row>
-    <row r="217" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="217" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D217" s="1"/>
       <c r="E217" s="1"/>
     </row>
-    <row r="219" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="219" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B219" s="2"/>
       <c r="C219" s="2"/>
     </row>
-    <row r="221" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="221" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D221" s="1"/>
       <c r="E221" s="1"/>
     </row>
-    <row r="223" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="223" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D223" s="1"/>
       <c r="E223" s="1"/>
     </row>
-    <row r="225" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="225" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D225" s="1"/>
       <c r="E225" s="1"/>
     </row>
-    <row r="232" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="232" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D232" s="1"/>
       <c r="E232" s="1"/>
     </row>
-    <row r="240" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="240" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C240" s="2"/>
       <c r="D240" s="2"/>
       <c r="E240" s="2"/>
     </row>
-    <row r="241" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="241" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B241" s="2"/>
       <c r="C241" s="2"/>
     </row>
-    <row r="256" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="256" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C256" s="2"/>
       <c r="D256" s="2"/>
       <c r="E256" s="2"/>
     </row>
-    <row r="258" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="258" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C258" s="2"/>
       <c r="D258" s="2"/>
       <c r="E258" s="2"/>
     </row>
-    <row r="259" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="259" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C259" s="2"/>
     </row>
-    <row r="265" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="265" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C265" s="2"/>
       <c r="D265" s="2"/>
       <c r="E265" s="2"/>
     </row>
-    <row r="269" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="269" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D269" s="1"/>
       <c r="E269" s="1"/>
     </row>
-    <row r="271" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="271" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C271" s="2"/>
     </row>
-    <row r="290" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="290" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C290" s="2"/>
       <c r="D290" s="2"/>
       <c r="E290" s="2"/>
     </row>
-    <row r="305" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="305" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D305" s="1"/>
       <c r="E305" s="1"/>
     </row>
-    <row r="368" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="368" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D368" s="1"/>
       <c r="E368" s="1"/>
     </row>
-    <row r="437" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="437" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D437" s="1"/>
       <c r="E437" s="1"/>
     </row>
-    <row r="438" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="438" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D438" s="1"/>
       <c r="E438" s="1"/>
     </row>
-    <row r="461" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="461" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C461" s="2"/>
       <c r="D461" s="2"/>
       <c r="E461" s="2"/>
     </row>
-    <row r="470" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="470" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C470" s="2"/>
       <c r="D470" s="2"/>
       <c r="E470" s="2"/>
     </row>
-    <row r="481" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="481" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C481" s="2"/>
       <c r="D481" s="2"/>
       <c r="E481" s="2"/>
     </row>
-    <row r="486" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="486" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D486" s="1"/>
       <c r="E486" s="1"/>
     </row>
-    <row r="487" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="487" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C487" s="2"/>
       <c r="D487" s="2"/>
       <c r="E487" s="2"/>
     </row>
-    <row r="488" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="488" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C488" s="2"/>
       <c r="D488" s="2"/>
       <c r="E488" s="2"/>
     </row>
-    <row r="493" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="493" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C493" s="2"/>
       <c r="D493" s="2"/>
       <c r="E493" s="2"/>
     </row>
-    <row r="495" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="495" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C495" s="2"/>
       <c r="D495" s="2"/>
       <c r="E495" s="2"/>
     </row>
-    <row r="499" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="499" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C499" s="2"/>
       <c r="D499" s="2"/>
       <c r="E499" s="2"/>
     </row>
-    <row r="500" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="500" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C500" s="2"/>
     </row>
-    <row r="509" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="509" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C509" s="2"/>
       <c r="D509" s="2"/>
       <c r="E509" s="2"/>
     </row>
-    <row r="523" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="523" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C523" s="2"/>
       <c r="D523" s="2"/>
       <c r="E523" s="2"/>
     </row>
-    <row r="524" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="524" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C524" s="2"/>
       <c r="D524" s="2"/>
       <c r="E524" s="2"/>
     </row>
-    <row r="525" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="525" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C525" s="2"/>
     </row>
-    <row r="536" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="536" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C536" s="2"/>
       <c r="D536" s="2"/>
       <c r="E536" s="2"/>
     </row>
-    <row r="544" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="544" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C544" s="2"/>
       <c r="D544" s="2"/>
       <c r="E544" s="2"/>
     </row>
-    <row r="555" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="555" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C555" s="2"/>
       <c r="D555" s="2"/>
       <c r="E555" s="2"/>
     </row>
-    <row r="566" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="566" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D566" s="1"/>
       <c r="E566" s="1"/>
     </row>
-    <row r="585" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="585" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C585" s="2"/>
       <c r="D585" s="2"/>
       <c r="E585" s="2"/>
     </row>
-    <row r="587" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="587" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C587" s="2"/>
       <c r="D587" s="2"/>
       <c r="E587" s="2"/>
     </row>
-    <row r="590" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="590" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D590" s="1"/>
       <c r="E590" s="1"/>
     </row>
-    <row r="594" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="594" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D594" s="1"/>
       <c r="E594" s="1"/>
     </row>
-    <row r="596" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="596" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C596" s="2"/>
       <c r="D596" s="2"/>
       <c r="E596" s="2"/>
     </row>
-    <row r="604" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="604" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C604" s="2"/>
       <c r="D604" s="2"/>
       <c r="E604" s="2"/>
     </row>
-    <row r="611" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="611" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C611" s="2"/>
       <c r="D611" s="2"/>
       <c r="E611" s="2"/>
     </row>
-    <row r="640" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="640" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D640" s="2"/>
       <c r="E640" s="2"/>
     </row>
-    <row r="658" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="658" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D658" s="1"/>
       <c r="E658" s="1"/>
     </row>
-    <row r="676" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="676" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C676" s="2"/>
       <c r="D676" s="2"/>
       <c r="E676" s="2"/>
     </row>
-    <row r="679" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="679" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C679" s="2"/>
       <c r="D679" s="2"/>
       <c r="E679" s="2"/>
     </row>
-    <row r="694" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="694" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D694" s="1"/>
       <c r="E694" s="1"/>
     </row>
-    <row r="730" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="730" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D730" s="1"/>
       <c r="E730" s="1"/>
     </row>
-    <row r="756" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="756" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C756" s="2"/>
     </row>
-    <row r="782" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="782" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D782" s="1"/>
       <c r="E782" s="1"/>
     </row>
-    <row r="788" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="788" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C788" s="2"/>
     </row>
-    <row r="851" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="851" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D851" s="1"/>
       <c r="E851" s="1"/>
     </row>
-    <row r="867" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="867" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D867" s="1"/>
       <c r="E867" s="1"/>
     </row>
-    <row r="877" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="877" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D877" s="1"/>
       <c r="E877" s="1"/>
     </row>
-    <row r="892" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="892" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D892" s="1"/>
       <c r="E892" s="1"/>
     </row>
@@ -1379,17 +1388,17 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="100.6640625" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.44140625" customWidth="1"/>
-    <col min="6" max="32" width="81.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="6" max="32" width="81.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
@@ -1403,7 +1412,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>75</v>
       </c>
@@ -1417,7 +1426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>74</v>
       </c>
@@ -1431,7 +1440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>73</v>
       </c>
@@ -1445,7 +1454,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>72</v>
       </c>
@@ -1459,7 +1468,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>71</v>
       </c>
@@ -1489,74 +1498,106 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="30.5546875" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="9.109375" style="4"/>
+    <col min="1" max="1" width="19.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" s="4">
+        <v>666</v>
+      </c>
+      <c r="D2" s="4">
+        <v>666</v>
+      </c>
+      <c r="E2" s="4">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" s="4">
+        <v>666</v>
+      </c>
+      <c r="D3" s="4">
+        <v>666</v>
+      </c>
+      <c r="E3" s="4">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="7"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="7"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
     </row>

</xml_diff>